<commit_message>
Modified code for sorting out ruminants
</commit_message>
<xml_diff>
--- a/min20-2022.05.16.xlsx
+++ b/min20-2022.05.16.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/walkermellon/cancerAcrossVertebrates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73dfa25a33a7cc34/Documents/GitHub/ruminants/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC0A390-FB83-B24C-89B4-0D644746317A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="3660" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="1680" windowWidth="24315" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="min20516 copy" sheetId="1" r:id="rId1"/>
@@ -4173,9 +4173,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4213,7 +4213,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4319,7 +4319,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4461,7 +4461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4471,13 +4471,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP328"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AQ1" sqref="AQ1:AQ1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2914</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>0.18569533799999999</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3941</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>0.21821789</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3124</v>
       </c>
@@ -4989,7 +4989,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3725</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>701</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>0.121267813</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2032</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>0.19245008999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2881</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>0.15617376199999999</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>117</v>
       </c>
@@ -5629,7 +5629,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2027</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>0.15811388300000001</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3076</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>8.0321932999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3645</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>5.3149399999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>17611</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>0.12700012699999999</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2215</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>8.3045480000000005E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2835</v>
       </c>
@@ -6397,7 +6397,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8028</v>
       </c>
@@ -6525,7 +6525,7 @@
         <v>0.17149858500000001</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1804</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>9.0909090999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4016</v>
       </c>
@@ -6781,7 +6781,7 @@
         <v>0.16903085100000001</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2618</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>0.16903085100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1155</v>
       </c>
@@ -7037,7 +7037,7 @@
         <v>0.10721125300000001</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1822</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>0.162221421</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1639</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>0.17677669500000001</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3765</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>0.21821789</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3020</v>
       </c>
@@ -7549,7 +7549,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3413</v>
       </c>
@@ -7677,7 +7677,7 @@
         <v>0.20412414500000001</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2521</v>
       </c>
@@ -7805,7 +7805,7 @@
         <v>0.108465229</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>897</v>
       </c>
@@ -7933,7 +7933,7 @@
         <v>0.145864991</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2926</v>
       </c>
@@ -8061,7 +8061,7 @@
         <v>0.141421356</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3922</v>
       </c>
@@ -8189,7 +8189,7 @@
         <v>6.9006555999999997E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3280</v>
       </c>
@@ -8317,7 +8317,7 @@
         <v>9.9503719000000004E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1543</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>0.188982237</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>14402</v>
       </c>
@@ -8573,7 +8573,7 @@
         <v>0.13867504899999999</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3278</v>
       </c>
@@ -8701,7 +8701,7 @@
         <v>0.110431526</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1386</v>
       </c>
@@ -8829,7 +8829,7 @@
         <v>0.182574186</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1226</v>
       </c>
@@ -8957,7 +8957,7 @@
         <v>0.15811388300000001</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4010</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>0.123091491</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>141</v>
       </c>
@@ -9213,7 +9213,7 @@
         <v>0.174077656</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3238</v>
       </c>
@@ -9341,7 +9341,7 @@
         <v>0.17149858500000001</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1828</v>
       </c>
@@ -9469,7 +9469,7 @@
         <v>0.18569533799999999</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>573</v>
       </c>
@@ -9597,7 +9597,7 @@
         <v>0.20412414500000001</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2888</v>
       </c>
@@ -9725,7 +9725,7 @@
         <v>9.7590007000000006E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1971</v>
       </c>
@@ -9853,7 +9853,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1245</v>
       </c>
@@ -9981,7 +9981,7 @@
         <v>0.17677669500000001</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4461</v>
       </c>
@@ -10109,7 +10109,7 @@
         <v>0.15617376199999999</v>
       </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3709</v>
       </c>
@@ -10237,7 +10237,7 @@
         <v>0.12909944500000001</v>
       </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2701</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>0.102062073</v>
       </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2601</v>
       </c>
@@ -10493,7 +10493,7 @@
         <v>0.13736056399999999</v>
       </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3078</v>
       </c>
@@ -10621,7 +10621,7 @@
         <v>0.19245008999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2699</v>
       </c>
@@ -10749,7 +10749,7 @@
         <v>0.120385853</v>
       </c>
     </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2698</v>
       </c>
@@ -10877,7 +10877,7 @@
         <v>0.11785113</v>
       </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3231</v>
       </c>
@@ -11005,7 +11005,7 @@
         <v>0.182574186</v>
       </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>893</v>
       </c>
@@ -11133,7 +11133,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2293</v>
       </c>
@@ -11261,7 +11261,7 @@
         <v>0.134839972</v>
       </c>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>11</v>
       </c>
@@ -11389,7 +11389,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="55" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>4101</v>
       </c>
@@ -11517,7 +11517,7 @@
         <v>0.21821789</v>
       </c>
     </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2670</v>
       </c>
@@ -11645,7 +11645,7 @@
         <v>0.131306433</v>
       </c>
     </row>
-    <row r="57" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3267</v>
       </c>
@@ -11773,7 +11773,7 @@
         <v>0.14744195600000001</v>
       </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4238</v>
       </c>
@@ -11901,7 +11901,7 @@
         <v>0.144337567</v>
       </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>3101</v>
       </c>
@@ -12029,7 +12029,7 @@
         <v>0.182574186</v>
       </c>
     </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>3596</v>
       </c>
@@ -12157,7 +12157,7 @@
         <v>0.15430335000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>98</v>
       </c>
@@ -12285,7 +12285,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="62" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3640</v>
       </c>
@@ -12413,7 +12413,7 @@
         <v>0.17149858500000001</v>
       </c>
     </row>
-    <row r="63" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2886</v>
       </c>
@@ -12541,7 +12541,7 @@
         <v>0.104257207</v>
       </c>
     </row>
-    <row r="64" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>90</v>
       </c>
@@ -12669,7 +12669,7 @@
         <v>0.182574186</v>
       </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3100</v>
       </c>
@@ -12797,7 +12797,7 @@
         <v>0.10721125300000001</v>
       </c>
     </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>950</v>
       </c>
@@ -12925,7 +12925,7 @@
         <v>9.2450033000000001E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>4505</v>
       </c>
@@ -13053,7 +13053,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>4471</v>
       </c>
@@ -13181,7 +13181,7 @@
         <v>0.144337567</v>
       </c>
     </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>4374</v>
       </c>
@@ -13309,7 +13309,7 @@
         <v>0.174077656</v>
       </c>
     </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>3711</v>
       </c>
@@ -13437,7 +13437,7 @@
         <v>0.17149858500000001</v>
       </c>
     </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>3712</v>
       </c>
@@ -13565,7 +13565,7 @@
         <v>0.118678166</v>
       </c>
     </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1657</v>
       </c>
@@ -13693,7 +13693,7 @@
         <v>0.20412414500000001</v>
       </c>
     </row>
-    <row r="73" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>3333</v>
       </c>
@@ -13821,7 +13821,7 @@
         <v>0.19245008999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1390</v>
       </c>
@@ -13949,7 +13949,7 @@
         <v>0.17149858500000001</v>
       </c>
     </row>
-    <row r="75" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>3268</v>
       </c>
@@ -14077,7 +14077,7 @@
         <v>0.11470786700000001</v>
       </c>
     </row>
-    <row r="76" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2621</v>
       </c>
@@ -14205,7 +14205,7 @@
         <v>0.15430335000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>4438</v>
       </c>
@@ -14333,7 +14333,7 @@
         <v>0.17960530199999999</v>
       </c>
     </row>
-    <row r="78" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2520</v>
       </c>
@@ -14461,7 +14461,7 @@
         <v>0.102597835</v>
       </c>
     </row>
-    <row r="79" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>952</v>
       </c>
@@ -14589,7 +14589,7 @@
         <v>0.16903085100000001</v>
       </c>
     </row>
-    <row r="80" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>3147</v>
       </c>
@@ -14717,7 +14717,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2722</v>
       </c>
@@ -14845,7 +14845,7 @@
         <v>0.17677669500000001</v>
       </c>
     </row>
-    <row r="82" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>936</v>
       </c>
@@ -14973,7 +14973,7 @@
         <v>0.16666666699999999</v>
       </c>
     </row>
-    <row r="83" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1270</v>
       </c>
@@ -15101,7 +15101,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="84" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2684</v>
       </c>
@@ -15229,7 +15229,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="85" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>63</v>
       </c>
@@ -15357,7 +15357,7 @@
         <v>0.11250879</v>
       </c>
     </row>
-    <row r="86" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2462</v>
       </c>
@@ -15485,7 +15485,7 @@
         <v>0.17149858500000001</v>
       </c>
     </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>3135</v>
       </c>
@@ -15613,7 +15613,7 @@
         <v>0.12909944500000001</v>
       </c>
     </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1097</v>
       </c>
@@ -15741,7 +15741,7 @@
         <v>0.15811388300000001</v>
       </c>
     </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2004</v>
       </c>
@@ -15869,7 +15869,7 @@
         <v>0.182574186</v>
       </c>
     </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1787</v>
       </c>
@@ -15997,7 +15997,7 @@
         <v>0.21821789</v>
       </c>
     </row>
-    <row r="91" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>4532</v>
       </c>
@@ -16125,7 +16125,7 @@
         <v>0.132453236</v>
       </c>
     </row>
-    <row r="92" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>3136</v>
       </c>
@@ -16253,7 +16253,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="93" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>3593</v>
       </c>
@@ -16381,7 +16381,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1524</v>
       </c>
@@ -16509,7 +16509,7 @@
         <v>0.182574186</v>
       </c>
     </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1647</v>
       </c>
@@ -16637,7 +16637,7 @@
         <v>0.17960530199999999</v>
       </c>
     </row>
-    <row r="96" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>12</v>
       </c>
@@ -16765,7 +16765,7 @@
         <v>0.118678166</v>
       </c>
     </row>
-    <row r="97" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>4422</v>
       </c>
@@ -16893,7 +16893,7 @@
         <v>0.196116135</v>
       </c>
     </row>
-    <row r="98" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2037</v>
       </c>
@@ -17021,7 +17021,7 @@
         <v>0.15811388300000001</v>
       </c>
     </row>
-    <row r="99" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>3127</v>
       </c>
@@ -17149,7 +17149,7 @@
         <v>0.196116135</v>
       </c>
     </row>
-    <row r="100" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>9</v>
       </c>
@@ -17277,7 +17277,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="101" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>4380</v>
       </c>
@@ -17405,7 +17405,7 @@
         <v>0.19245008999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>4379</v>
       </c>
@@ -17533,7 +17533,7 @@
         <v>0.188982237</v>
       </c>
     </row>
-    <row r="103" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1854</v>
       </c>
@@ -17661,7 +17661,7 @@
         <v>0.16903085100000001</v>
       </c>
     </row>
-    <row r="104" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>3863</v>
       </c>
@@ -17789,7 +17789,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="105" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>3635</v>
       </c>
@@ -17917,7 +17917,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="106" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1415</v>
       </c>
@@ -18045,7 +18045,7 @@
         <v>0.13018891099999999</v>
       </c>
     </row>
-    <row r="107" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1471</v>
       </c>
@@ -18173,7 +18173,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="108" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>3304</v>
       </c>
@@ -18301,7 +18301,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="109" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>11488</v>
       </c>
@@ -18429,7 +18429,7 @@
         <v>0.12803687999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>3334</v>
       </c>
@@ -18557,7 +18557,7 @@
         <v>0.105999788</v>
       </c>
     </row>
-    <row r="111" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2486</v>
       </c>
@@ -18685,7 +18685,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="112" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>3575</v>
       </c>
@@ -18813,7 +18813,7 @@
         <v>0.19245008999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>3288</v>
       </c>
@@ -18941,7 +18941,7 @@
         <v>0.14002800800000001</v>
       </c>
     </row>
-    <row r="114" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>495</v>
       </c>
@@ -19069,7 +19069,7 @@
         <v>0.21821789</v>
       </c>
     </row>
-    <row r="115" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>3582</v>
       </c>
@@ -19197,7 +19197,7 @@
         <v>0.144337567</v>
       </c>
     </row>
-    <row r="116" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>3572</v>
       </c>
@@ -19325,7 +19325,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="117" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1148</v>
       </c>
@@ -19453,7 +19453,7 @@
         <v>0.144337567</v>
       </c>
     </row>
-    <row r="118" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2077</v>
       </c>
@@ -19581,7 +19581,7 @@
         <v>0.21821789</v>
       </c>
     </row>
-    <row r="119" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1940</v>
       </c>
@@ -19709,7 +19709,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="120" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>3691</v>
       </c>
@@ -19837,7 +19837,7 @@
         <v>0.111803399</v>
       </c>
     </row>
-    <row r="121" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>4092</v>
       </c>
@@ -19965,7 +19965,7 @@
         <v>0.20412414500000001</v>
       </c>
     </row>
-    <row r="122" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2883</v>
       </c>
@@ -20093,7 +20093,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="123" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>295</v>
       </c>
@@ -20221,7 +20221,7 @@
         <v>0.15249857</v>
       </c>
     </row>
-    <row r="124" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>1829</v>
       </c>
@@ -20349,7 +20349,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="125" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>4046</v>
       </c>
@@ -20477,7 +20477,7 @@
         <v>0.15617376199999999</v>
       </c>
     </row>
-    <row r="126" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>399</v>
       </c>
@@ -20605,7 +20605,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="127" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2634</v>
       </c>
@@ -20733,7 +20733,7 @@
         <v>9.5346259000000003E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>780</v>
       </c>
@@ -20861,7 +20861,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="129" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2041</v>
       </c>
@@ -20989,7 +20989,7 @@
         <v>0.188982237</v>
       </c>
     </row>
-    <row r="130" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>18222</v>
       </c>
@@ -21117,7 +21117,7 @@
         <v>0.113227703</v>
       </c>
     </row>
-    <row r="131" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>80</v>
       </c>
@@ -21245,7 +21245,7 @@
         <v>0.15249857</v>
       </c>
     </row>
-    <row r="132" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>11776</v>
       </c>
@@ -21373,7 +21373,7 @@
         <v>0.145864991</v>
       </c>
     </row>
-    <row r="133" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>3257</v>
       </c>
@@ -21501,7 +21501,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="134" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2706</v>
       </c>
@@ -21629,7 +21629,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="135" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>647</v>
       </c>
@@ -21757,7 +21757,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="136" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>1800</v>
       </c>
@@ -21885,7 +21885,7 @@
         <v>0.133630621</v>
       </c>
     </row>
-    <row r="137" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>4273</v>
       </c>
@@ -22013,7 +22013,7 @@
         <v>0.111803399</v>
       </c>
     </row>
-    <row r="138" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>1878</v>
       </c>
@@ -22141,7 +22141,7 @@
         <v>0.21821789</v>
       </c>
     </row>
-    <row r="139" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>1559</v>
       </c>
@@ -22269,7 +22269,7 @@
         <v>0.111803399</v>
       </c>
     </row>
-    <row r="140" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>10572</v>
       </c>
@@ -22397,7 +22397,7 @@
         <v>0.17677669500000001</v>
       </c>
     </row>
-    <row r="141" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2644</v>
       </c>
@@ -22525,7 +22525,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="142" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2624</v>
       </c>
@@ -22653,7 +22653,7 @@
         <v>0.17960530199999999</v>
       </c>
     </row>
-    <row r="143" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>1915</v>
       </c>
@@ -22781,7 +22781,7 @@
         <v>0.14907119799999999</v>
       </c>
     </row>
-    <row r="144" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>4124</v>
       </c>
@@ -22909,7 +22909,7 @@
         <v>0.17149858500000001</v>
       </c>
     </row>
-    <row r="145" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>8225</v>
       </c>
@@ -23037,7 +23037,7 @@
         <v>0.188982237</v>
       </c>
     </row>
-    <row r="146" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>2643</v>
       </c>
@@ -23165,7 +23165,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="147" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>810</v>
       </c>
@@ -23293,7 +23293,7 @@
         <v>0.182574186</v>
       </c>
     </row>
-    <row r="148" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>1315</v>
       </c>
@@ -23421,7 +23421,7 @@
         <v>0.15617376199999999</v>
       </c>
     </row>
-    <row r="149" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>3566</v>
       </c>
@@ -23549,7 +23549,7 @@
         <v>0.12803687999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>3687</v>
       </c>
@@ -23677,7 +23677,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="151" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>8200</v>
       </c>
@@ -23805,7 +23805,7 @@
         <v>0.11785113</v>
       </c>
     </row>
-    <row r="152" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>1606</v>
       </c>
@@ -23933,7 +23933,7 @@
         <v>0.18569533799999999</v>
       </c>
     </row>
-    <row r="153" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>5246</v>
       </c>
@@ -24061,7 +24061,7 @@
         <v>0.16666666699999999</v>
       </c>
     </row>
-    <row r="154" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>4166</v>
       </c>
@@ -24189,7 +24189,7 @@
         <v>0.123091491</v>
       </c>
     </row>
-    <row r="155" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>1210</v>
       </c>
@@ -24317,7 +24317,7 @@
         <v>0.20412414500000001</v>
       </c>
     </row>
-    <row r="156" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>15239</v>
       </c>
@@ -24445,7 +24445,7 @@
         <v>0.117041147</v>
       </c>
     </row>
-    <row r="157" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>542</v>
       </c>
@@ -24573,7 +24573,7 @@
         <v>0.16012815399999999</v>
       </c>
     </row>
-    <row r="158" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>918</v>
       </c>
@@ -24701,7 +24701,7 @@
         <v>0.174077656</v>
       </c>
     </row>
-    <row r="159" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>1196</v>
       </c>
@@ -24829,7 +24829,7 @@
         <v>0.102062073</v>
       </c>
     </row>
-    <row r="160" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>19344</v>
       </c>
@@ -24957,7 +24957,7 @@
         <v>0.196116135</v>
       </c>
     </row>
-    <row r="161" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>19342</v>
       </c>
@@ -25085,7 +25085,7 @@
         <v>6.8041381999999997E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>368</v>
       </c>
@@ -25213,7 +25213,7 @@
         <v>0.15430335000000001</v>
       </c>
     </row>
-    <row r="163" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>412</v>
       </c>
@@ -25341,7 +25341,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="164" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>823</v>
       </c>
@@ -25469,7 +25469,7 @@
         <v>0.162221421</v>
       </c>
     </row>
-    <row r="165" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>1083</v>
       </c>
@@ -25597,7 +25597,7 @@
         <v>0.19245008999999999</v>
       </c>
     </row>
-    <row r="166" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>1360</v>
       </c>
@@ -25725,7 +25725,7 @@
         <v>0.20412414500000001</v>
       </c>
     </row>
-    <row r="167" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>1532</v>
       </c>
@@ -25853,7 +25853,7 @@
         <v>0.174077656</v>
       </c>
     </row>
-    <row r="168" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>2395</v>
       </c>
@@ -25981,7 +25981,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="169" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2487</v>
       </c>
@@ -26109,7 +26109,7 @@
         <v>0.20412414500000001</v>
       </c>
     </row>
-    <row r="170" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>2595</v>
       </c>
@@ -26237,7 +26237,7 @@
         <v>0.16012815399999999</v>
       </c>
     </row>
-    <row r="171" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>2785</v>
       </c>
@@ -26365,7 +26365,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="172" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>19426</v>
       </c>
@@ -26493,7 +26493,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="173" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>3004</v>
       </c>
@@ -26621,7 +26621,7 @@
         <v>0.182574186</v>
       </c>
     </row>
-    <row r="174" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>3296</v>
       </c>
@@ -26749,7 +26749,7 @@
         <v>0.141421356</v>
       </c>
     </row>
-    <row r="175" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>3297</v>
       </c>
@@ -26877,7 +26877,7 @@
         <v>0.164398987</v>
       </c>
     </row>
-    <row r="176" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>3299</v>
       </c>
@@ -27005,7 +27005,7 @@
         <v>0.11952286099999999</v>
       </c>
     </row>
-    <row r="177" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>4261</v>
       </c>
@@ -27133,7 +27133,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="178" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>4358</v>
       </c>
@@ -27261,7 +27261,7 @@
         <v>0.15430335000000001</v>
       </c>
     </row>
-    <row r="179" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>4361</v>
       </c>
@@ -27389,7 +27389,7 @@
         <v>0.15811388300000001</v>
       </c>
     </row>
-    <row r="180" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>4403</v>
       </c>
@@ -27517,7 +27517,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="181" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>4478</v>
       </c>
@@ -27645,7 +27645,7 @@
         <v>0.19245008999999999</v>
       </c>
     </row>
-    <row r="182" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>19619</v>
       </c>
@@ -27773,7 +27773,7 @@
         <v>0.122169444</v>
       </c>
     </row>
-    <row r="183" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>2726</v>
       </c>
@@ -27901,7 +27901,7 @@
         <v>5.7353933000000003E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>572</v>
       </c>
@@ -28029,7 +28029,7 @@
         <v>8.5435765999999996E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>1649</v>
       </c>
@@ -28157,7 +28157,7 @@
         <v>6.1199006E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>3923</v>
       </c>
@@ -28285,7 +28285,7 @@
         <v>5.1571062000000001E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>2941</v>
       </c>
@@ -28413,7 +28413,7 @@
         <v>7.6028592000000006E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>3639</v>
       </c>
@@ -28541,7 +28541,7 @@
         <v>0.11470786700000001</v>
       </c>
     </row>
-    <row r="189" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>1767</v>
       </c>
@@ -28669,7 +28669,7 @@
         <v>0.12909944500000001</v>
       </c>
     </row>
-    <row r="190" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>1398</v>
       </c>
@@ -28797,7 +28797,7 @@
         <v>0.134839972</v>
       </c>
     </row>
-    <row r="191" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>120</v>
       </c>
@@ -28925,7 +28925,7 @@
         <v>9.6225044999999995E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>1468</v>
       </c>
@@ -29053,7 +29053,7 @@
         <v>0.13736056399999999</v>
       </c>
     </row>
-    <row r="193" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>1293</v>
       </c>
@@ -29181,7 +29181,7 @@
         <v>0.144337567</v>
       </c>
     </row>
-    <row r="194" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>576</v>
       </c>
@@ -29309,7 +29309,7 @@
         <v>0.15075567200000001</v>
       </c>
     </row>
-    <row r="195" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>1656</v>
       </c>
@@ -29437,7 +29437,7 @@
         <v>0.109108945</v>
       </c>
     </row>
-    <row r="196" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>675</v>
       </c>
@@ -29565,7 +29565,7 @@
         <v>0.10976426</v>
       </c>
     </row>
-    <row r="197" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>2695</v>
       </c>
@@ -29693,7 +29693,7 @@
         <v>0.15617376199999999</v>
       </c>
     </row>
-    <row r="198" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>314</v>
       </c>
@@ -29821,7 +29821,7 @@
         <v>7.0710677999999999E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>4272</v>
       </c>
@@ -29949,7 +29949,7 @@
         <v>7.2547625000000004E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>2404</v>
       </c>
@@ -30077,7 +30077,7 @@
         <v>0.164398987</v>
       </c>
     </row>
-    <row r="201" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>111</v>
       </c>
@@ -30205,7 +30205,7 @@
         <v>0.117041147</v>
       </c>
     </row>
-    <row r="202" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>4547</v>
       </c>
@@ -30333,7 +30333,7 @@
         <v>0.16903085100000001</v>
       </c>
     </row>
-    <row r="203" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>3706</v>
       </c>
@@ -30461,7 +30461,7 @@
         <v>0.16903085100000001</v>
       </c>
     </row>
-    <row r="204" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>1827</v>
       </c>
@@ -30589,7 +30589,7 @@
         <v>9.7590007000000006E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>3173</v>
       </c>
@@ -30717,7 +30717,7 @@
         <v>0.17149858500000001</v>
       </c>
     </row>
-    <row r="206" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>2492</v>
       </c>
@@ -30845,7 +30845,7 @@
         <v>0.17149858500000001</v>
       </c>
     </row>
-    <row r="207" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>4333</v>
       </c>
@@ -30973,7 +30973,7 @@
         <v>0.17149858500000001</v>
       </c>
     </row>
-    <row r="208" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>3372</v>
       </c>
@@ -31101,7 +31101,7 @@
         <v>0.174077656</v>
       </c>
     </row>
-    <row r="209" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>2958</v>
       </c>
@@ -31229,7 +31229,7 @@
         <v>0.174077656</v>
       </c>
     </row>
-    <row r="210" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>2296</v>
       </c>
@@ -31357,7 +31357,7 @@
         <v>0.174077656</v>
       </c>
     </row>
-    <row r="211" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>4051</v>
       </c>
@@ -31485,7 +31485,7 @@
         <v>0.17677669500000001</v>
       </c>
     </row>
-    <row r="212" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>140</v>
       </c>
@@ -31613,7 +31613,7 @@
         <v>0.17677669500000001</v>
       </c>
     </row>
-    <row r="213" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>1029</v>
       </c>
@@ -31741,7 +31741,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="214" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>2391</v>
       </c>
@@ -31869,7 +31869,7 @@
         <v>0.17677669500000001</v>
       </c>
     </row>
-    <row r="215" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>4156</v>
       </c>
@@ -31997,7 +31997,7 @@
         <v>0.17677669500000001</v>
       </c>
     </row>
-    <row r="216" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>4416</v>
       </c>
@@ -32125,7 +32125,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="217" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>1860</v>
       </c>
@@ -32253,7 +32253,7 @@
         <v>0.17960530199999999</v>
       </c>
     </row>
-    <row r="218" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>1723</v>
       </c>
@@ -32381,7 +32381,7 @@
         <v>0.17960530199999999</v>
       </c>
     </row>
-    <row r="219" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>3194</v>
       </c>
@@ -32509,7 +32509,7 @@
         <v>0.17960530199999999</v>
       </c>
     </row>
-    <row r="220" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>1419</v>
       </c>
@@ -32637,7 +32637,7 @@
         <v>0.18569533799999999</v>
       </c>
     </row>
-    <row r="221" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>2313</v>
       </c>
@@ -32765,7 +32765,7 @@
         <v>0.18569533799999999</v>
       </c>
     </row>
-    <row r="222" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>4052</v>
       </c>
@@ -32893,7 +32893,7 @@
         <v>0.18569533799999999</v>
       </c>
     </row>
-    <row r="223" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>3750</v>
       </c>
@@ -33021,7 +33021,7 @@
         <v>0.133630621</v>
       </c>
     </row>
-    <row r="224" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>540</v>
       </c>
@@ -33149,7 +33149,7 @@
         <v>0.134839972</v>
       </c>
     </row>
-    <row r="225" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>4414</v>
       </c>
@@ -33277,7 +33277,7 @@
         <v>0.134839972</v>
       </c>
     </row>
-    <row r="226" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>1519</v>
       </c>
@@ -33405,7 +33405,7 @@
         <v>0.19245008999999999</v>
       </c>
     </row>
-    <row r="227" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>3324</v>
       </c>
@@ -33533,7 +33533,7 @@
         <v>9.6225044999999995E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>4165</v>
       </c>
@@ -33661,7 +33661,7 @@
         <v>0.196116135</v>
       </c>
     </row>
-    <row r="229" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>2700</v>
       </c>
@@ -33789,7 +33789,7 @@
         <v>0.11396057599999999</v>
       </c>
     </row>
-    <row r="230" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>3633</v>
       </c>
@@ -33917,7 +33917,7 @@
         <v>9.9014753999999996E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>1984</v>
       </c>
@@ -34045,7 +34045,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="232" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>2867</v>
       </c>
@@ -34173,7 +34173,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="233" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>1527</v>
       </c>
@@ -34301,7 +34301,7 @@
         <v>0.14285714299999999</v>
       </c>
     </row>
-    <row r="234" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>2858</v>
       </c>
@@ -34429,7 +34429,7 @@
         <v>0.20412414500000001</v>
       </c>
     </row>
-    <row r="235" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>2985</v>
       </c>
@@ -34557,7 +34557,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="236" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>282</v>
       </c>
@@ -34685,7 +34685,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="237" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>4463</v>
       </c>
@@ -34813,7 +34813,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="238" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>1991</v>
       </c>
@@ -34941,7 +34941,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="239" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>1745</v>
       </c>
@@ -35069,7 +35069,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="240" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>3695</v>
       </c>
@@ -35197,7 +35197,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="241" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>3196</v>
       </c>
@@ -35325,7 +35325,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="242" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>1397</v>
       </c>
@@ -35453,7 +35453,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="243" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>1660</v>
       </c>
@@ -35581,7 +35581,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="244" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>1626</v>
       </c>
@@ -35709,7 +35709,7 @@
         <v>0.15430335000000001</v>
       </c>
     </row>
-    <row r="245" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>2516</v>
       </c>
@@ -35837,7 +35837,7 @@
         <v>0.15430335000000001</v>
       </c>
     </row>
-    <row r="246" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>2869</v>
       </c>
@@ -35965,7 +35965,7 @@
         <v>0.12598815799999999</v>
       </c>
     </row>
-    <row r="247" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>1774</v>
       </c>
@@ -36093,7 +36093,7 @@
         <v>0.15430335000000001</v>
       </c>
     </row>
-    <row r="248" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>3777</v>
       </c>
@@ -36221,7 +36221,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="249" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>4360</v>
       </c>
@@ -36349,7 +36349,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="250" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>2132</v>
       </c>
@@ -36477,7 +36477,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="251" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>857</v>
       </c>
@@ -36605,7 +36605,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="252" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>1640</v>
       </c>
@@ -36733,7 +36733,7 @@
         <v>0.113227703</v>
       </c>
     </row>
-    <row r="253" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>3959</v>
       </c>
@@ -36861,7 +36861,7 @@
         <v>0.162221421</v>
       </c>
     </row>
-    <row r="254" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>1</v>
       </c>
@@ -36989,7 +36989,7 @@
         <v>0.162221421</v>
       </c>
     </row>
-    <row r="255" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>2588</v>
       </c>
@@ -37117,7 +37117,7 @@
         <v>0.164398987</v>
       </c>
     </row>
-    <row r="256" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>3545</v>
       </c>
@@ -37245,7 +37245,7 @@
         <v>0.136082763</v>
       </c>
     </row>
-    <row r="257" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>1425</v>
       </c>
@@ -37373,7 +37373,7 @@
         <v>0.136082763</v>
       </c>
     </row>
-    <row r="258" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>1435</v>
       </c>
@@ -37501,7 +37501,7 @@
         <v>0.105999788</v>
       </c>
     </row>
-    <row r="259" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>3375</v>
       </c>
@@ -37629,7 +37629,7 @@
         <v>0.16903085100000001</v>
       </c>
     </row>
-    <row r="260" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>3111</v>
       </c>
@@ -37757,7 +37757,7 @@
         <v>0.17149858500000001</v>
       </c>
     </row>
-    <row r="261" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>3670</v>
       </c>
@@ -37885,7 +37885,7 @@
         <v>0.174077656</v>
       </c>
     </row>
-    <row r="262" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>538</v>
       </c>
@@ -38013,7 +38013,7 @@
         <v>0.111803399</v>
       </c>
     </row>
-    <row r="263" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>2704</v>
       </c>
@@ -38141,7 +38141,7 @@
         <v>0.12598815799999999</v>
       </c>
     </row>
-    <row r="264" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>1005</v>
       </c>
@@ -38269,7 +38269,7 @@
         <v>6.7573737999999994E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>223</v>
       </c>
@@ -38397,7 +38397,7 @@
         <v>0.117041147</v>
       </c>
     </row>
-    <row r="266" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>1830</v>
       </c>
@@ -38525,7 +38525,7 @@
         <v>0.18569533799999999</v>
       </c>
     </row>
-    <row r="267" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>2551</v>
       </c>
@@ -38653,7 +38653,7 @@
         <v>0.188982237</v>
       </c>
     </row>
-    <row r="268" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>3734</v>
       </c>
@@ -38781,7 +38781,7 @@
         <v>0.15617376199999999</v>
       </c>
     </row>
-    <row r="269" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>3387</v>
       </c>
@@ -38909,7 +38909,7 @@
         <v>0.19245008999999999</v>
       </c>
     </row>
-    <row r="270" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>1710</v>
       </c>
@@ -39037,7 +39037,7 @@
         <v>0.136082763</v>
       </c>
     </row>
-    <row r="271" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>3907</v>
       </c>
@@ -39165,7 +39165,7 @@
         <v>0.19245008999999999</v>
       </c>
     </row>
-    <row r="272" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>407</v>
       </c>
@@ -39293,7 +39293,7 @@
         <v>0.162221421</v>
       </c>
     </row>
-    <row r="273" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>737</v>
       </c>
@@ -39421,7 +39421,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="274" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>1388</v>
       </c>
@@ -39549,7 +39549,7 @@
         <v>0.164398987</v>
       </c>
     </row>
-    <row r="275" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>3470</v>
       </c>
@@ -39677,7 +39677,7 @@
         <v>8.2199493999999998E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>3472</v>
       </c>
@@ -39805,7 +39805,7 @@
         <v>0.164398987</v>
       </c>
     </row>
-    <row r="277" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>825</v>
       </c>
@@ -39933,7 +39933,7 @@
         <v>6.6519011000000003E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>1652</v>
       </c>
@@ -40061,7 +40061,7 @@
         <v>8.7705801999999999E-2</v>
       </c>
     </row>
-    <row r="279" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>2871</v>
       </c>
@@ -40189,7 +40189,7 @@
         <v>0.145864991</v>
       </c>
     </row>
-    <row r="280" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>3204</v>
       </c>
@@ -40317,7 +40317,7 @@
         <v>0.20851441400000001</v>
       </c>
     </row>
-    <row r="281" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>4217</v>
       </c>
@@ -40445,7 +40445,7 @@
         <v>0.120385853</v>
       </c>
     </row>
-    <row r="282" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>2594</v>
       </c>
@@ -40573,7 +40573,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="283" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>680</v>
       </c>
@@ -40701,7 +40701,7 @@
         <v>0.17677669500000001</v>
       </c>
     </row>
-    <row r="284" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>3252</v>
       </c>
@@ -40829,7 +40829,7 @@
         <v>0.21821789</v>
       </c>
     </row>
-    <row r="285" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>3879</v>
       </c>
@@ -40957,7 +40957,7 @@
         <v>0.21821789</v>
       </c>
     </row>
-    <row r="286" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>125</v>
       </c>
@@ -41085,7 +41085,7 @@
         <v>0.21821789</v>
       </c>
     </row>
-    <row r="287" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>347</v>
       </c>
@@ -41213,7 +41213,7 @@
         <v>0.17960530199999999</v>
       </c>
     </row>
-    <row r="288" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>1930</v>
       </c>
@@ -41341,7 +41341,7 @@
         <v>0.15617376199999999</v>
       </c>
     </row>
-    <row r="289" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>1706</v>
       </c>
@@ -41469,7 +41469,7 @@
         <v>0.14744195600000001</v>
       </c>
     </row>
-    <row r="290" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>2780</v>
       </c>
@@ -41597,7 +41597,7 @@
         <v>0.16666666699999999</v>
       </c>
     </row>
-    <row r="291" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>2610</v>
       </c>
@@ -41725,7 +41725,7 @@
         <v>0.12598815799999999</v>
       </c>
     </row>
-    <row r="292" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>679</v>
       </c>
@@ -41853,7 +41853,7 @@
         <v>0.16903085100000001</v>
       </c>
     </row>
-    <row r="293" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>3019</v>
       </c>
@@ -41981,7 +41981,7 @@
         <v>0.11952286099999999</v>
       </c>
     </row>
-    <row r="294" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>2570</v>
       </c>
@@ -42109,7 +42109,7 @@
         <v>0.13867504899999999</v>
       </c>
     </row>
-    <row r="295" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>2159</v>
       </c>
@@ -42237,7 +42237,7 @@
         <v>0.174077656</v>
       </c>
     </row>
-    <row r="296" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>3694</v>
       </c>
@@ -42365,7 +42365,7 @@
         <v>0.132453236</v>
       </c>
     </row>
-    <row r="297" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>84</v>
       </c>
@@ -42493,7 +42493,7 @@
         <v>0.16012815399999999</v>
       </c>
     </row>
-    <row r="298" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>2804</v>
       </c>
@@ -42621,7 +42621,7 @@
         <v>0.118678166</v>
       </c>
     </row>
-    <row r="299" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>119</v>
       </c>
@@ -42749,7 +42749,7 @@
         <v>0.188982237</v>
       </c>
     </row>
-    <row r="300" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>3665</v>
       </c>
@@ -42877,7 +42877,7 @@
         <v>0.21821789</v>
       </c>
     </row>
-    <row r="301" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>2984</v>
       </c>
@@ -43005,7 +43005,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="302" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>1526</v>
       </c>
@@ -43133,7 +43133,7 @@
         <v>0.196116135</v>
       </c>
     </row>
-    <row r="303" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>1025</v>
       </c>
@@ -43261,7 +43261,7 @@
         <v>9.5782628999999994E-2</v>
       </c>
     </row>
-    <row r="304" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>4007</v>
       </c>
@@ -43389,7 +43389,7 @@
         <v>8.6710996999999998E-2</v>
       </c>
     </row>
-    <row r="305" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>3013</v>
       </c>
@@ -43517,7 +43517,7 @@
         <v>0.136082763</v>
       </c>
     </row>
-    <row r="306" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>1175</v>
       </c>
@@ -43645,7 +43645,7 @@
         <v>0.20412414500000001</v>
       </c>
     </row>
-    <row r="307" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>3402</v>
       </c>
@@ -43773,7 +43773,7 @@
         <v>0.13018891099999999</v>
       </c>
     </row>
-    <row r="308" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>2160</v>
       </c>
@@ -43901,7 +43901,7 @@
         <v>0.12598815799999999</v>
       </c>
     </row>
-    <row r="309" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>72</v>
       </c>
@@ -44029,7 +44029,7 @@
         <v>0.21320071600000001</v>
       </c>
     </row>
-    <row r="310" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>357</v>
       </c>
@@ -44157,7 +44157,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="311" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>226</v>
       </c>
@@ -44285,7 +44285,7 @@
         <v>0.223606798</v>
       </c>
     </row>
-    <row r="312" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>686</v>
       </c>
@@ -44413,7 +44413,7 @@
         <v>0.134839972</v>
       </c>
     </row>
-    <row r="313" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>2807</v>
       </c>
@@ -44541,7 +44541,7 @@
         <v>4.5786855000000001E-2</v>
       </c>
     </row>
-    <row r="314" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>1612</v>
       </c>
@@ -44669,7 +44669,7 @@
         <v>8.5435765999999996E-2</v>
       </c>
     </row>
-    <row r="315" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>301</v>
       </c>
@@ -44797,7 +44797,7 @@
         <v>0.174077656</v>
       </c>
     </row>
-    <row r="316" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>514</v>
       </c>
@@ -44925,7 +44925,7 @@
         <v>0.15430335000000001</v>
       </c>
     </row>
-    <row r="317" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>4180</v>
       </c>
@@ -45053,7 +45053,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="318" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>1946</v>
       </c>
@@ -45181,7 +45181,7 @@
         <v>6.0633906000000001E-2</v>
       </c>
     </row>
-    <row r="319" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>3247</v>
       </c>
@@ -45309,7 +45309,7 @@
         <v>0.109108945</v>
       </c>
     </row>
-    <row r="320" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>3340</v>
       </c>
@@ -45437,7 +45437,7 @@
         <v>0.17960530199999999</v>
       </c>
     </row>
-    <row r="321" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>2470</v>
       </c>
@@ -45565,7 +45565,7 @@
         <v>0.174077656</v>
       </c>
     </row>
-    <row r="322" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>3615</v>
       </c>
@@ -45693,7 +45693,7 @@
         <v>0.20412414500000001</v>
       </c>
     </row>
-    <row r="323" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>3140</v>
       </c>
@@ -45821,7 +45821,7 @@
         <v>0.122169444</v>
       </c>
     </row>
-    <row r="324" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>7</v>
       </c>
@@ -45940,7 +45940,7 @@
         <v>0.15641797199999999</v>
       </c>
     </row>
-    <row r="325" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>3335</v>
       </c>
@@ -46068,7 +46068,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="326" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>2475</v>
       </c>
@@ -46196,7 +46196,7 @@
         <v>0.14744195600000001</v>
       </c>
     </row>
-    <row r="327" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>565</v>
       </c>
@@ -46324,7 +46324,7 @@
         <v>8.2478609999999994E-2</v>
       </c>
     </row>
-    <row r="328" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>2550</v>
       </c>
@@ -46461,17 +46461,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1150</v>
       </c>
@@ -46479,7 +46479,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1152</v>
       </c>
@@ -46487,7 +46487,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -46495,7 +46495,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1155</v>
       </c>
@@ -46503,7 +46503,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -46511,7 +46511,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -46519,7 +46519,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -46527,7 +46527,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1160</v>
       </c>
@@ -46535,7 +46535,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -46543,7 +46543,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -46551,7 +46551,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -46559,7 +46559,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -46567,7 +46567,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -46575,7 +46575,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -46583,7 +46583,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -46591,7 +46591,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
@@ -46599,7 +46599,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -46607,7 +46607,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -46615,7 +46615,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -46623,7 +46623,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -46631,7 +46631,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -46639,7 +46639,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -46647,7 +46647,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -46655,7 +46655,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -46663,7 +46663,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -46671,7 +46671,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -46679,7 +46679,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -46687,7 +46687,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -46695,7 +46695,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -46703,7 +46703,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -46711,7 +46711,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -46719,7 +46719,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -46727,7 +46727,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -46735,7 +46735,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -46743,7 +46743,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -46751,7 +46751,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -46759,7 +46759,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -46767,7 +46767,7 @@
         <v>1189</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -46775,7 +46775,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -46783,7 +46783,7 @@
         <v>1191</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>

</xml_diff>